<commit_message>
move solver to subfolder
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hardware\63_Glowing_Polyhedrons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{48AA3F5A-3296-4F6D-A56C-8299F12BD58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA725455-B396-4ADB-8D04-E6B6323D60C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{5BF2D058-20B1-4E68-B932-3EECD9DE5D4B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="21">
   <si>
     <t>Cube</t>
   </si>
@@ -36,9 +36,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>Full coverage with equal current</t>
-  </si>
-  <si>
     <t>Triangular Prism</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>Dodecahedron</t>
   </si>
   <si>
-    <t xml:space="preserve">Path length </t>
-  </si>
-  <si>
     <t>Vertices</t>
   </si>
   <si>
@@ -88,6 +82,12 @@
   </si>
   <si>
     <t>Stellated Octahedron</t>
+  </si>
+  <si>
+    <t>L=1</t>
+  </si>
+  <si>
+    <t>Taps for full coverage, equal current</t>
   </si>
 </sst>
 </file>
@@ -530,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2730FE3-BE20-49D8-AF28-F682CEA2B90A}">
-  <dimension ref="D2:K21"/>
+  <dimension ref="D5:Y21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K18"/>
+      <selection activeCell="X11" sqref="X11:X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,29 +542,31 @@
     <col min="7" max="9" width="8.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:25" x14ac:dyDescent="0.3">
       <c r="G5" s="11" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
-    </row>
-    <row r="6" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="O5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+    </row>
+    <row r="6" spans="4:25" x14ac:dyDescent="0.3">
       <c r="E6" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="H6" s="1">
         <v>2</v>
@@ -578,8 +580,41 @@
       <c r="K6" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="O6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P6" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>3</v>
+      </c>
+      <c r="R6" s="1">
+        <v>4</v>
+      </c>
+      <c r="S6" s="1">
+        <v>5</v>
+      </c>
+      <c r="T6" s="1">
+        <v>6</v>
+      </c>
+      <c r="U6" s="1">
+        <v>7</v>
+      </c>
+      <c r="V6" s="1">
+        <v>8</v>
+      </c>
+      <c r="W6" s="1">
+        <v>9</v>
+      </c>
+      <c r="X6" s="1">
+        <v>10</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="4:25" x14ac:dyDescent="0.3">
       <c r="D7" s="9" t="s">
         <v>1</v>
       </c>
@@ -605,9 +640,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:25" x14ac:dyDescent="0.3">
       <c r="D8" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8" s="5">
         <v>6</v>
@@ -631,7 +666,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:25" x14ac:dyDescent="0.3">
       <c r="D9" s="9" t="s">
         <v>0</v>
       </c>
@@ -657,9 +692,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:25" x14ac:dyDescent="0.3">
       <c r="D10" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10" s="5">
         <v>6</v>
@@ -683,9 +718,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:25" x14ac:dyDescent="0.3">
       <c r="D11" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11" s="5">
         <v>10</v>
@@ -709,9 +744,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:25" x14ac:dyDescent="0.3">
       <c r="D12" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12" s="5">
         <v>12</v>
@@ -735,9 +770,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:25" x14ac:dyDescent="0.3">
       <c r="D13" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" s="5">
         <v>8</v>
@@ -761,9 +796,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:25" x14ac:dyDescent="0.3">
       <c r="D14" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" s="5">
         <v>12</v>
@@ -787,9 +822,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:25" x14ac:dyDescent="0.3">
       <c r="D15" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" s="5">
         <v>12</v>
@@ -813,9 +848,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:25" x14ac:dyDescent="0.3">
       <c r="D16" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E16" s="5">
         <v>14</v>
@@ -841,7 +876,7 @@
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D17" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E17" s="5">
         <v>11</v>
@@ -867,7 +902,7 @@
     </row>
     <row r="18" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D18" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E18" s="5">
         <v>20</v>
@@ -876,13 +911,13 @@
         <v>30</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J18" s="7" t="s">
         <v>2</v>
@@ -893,7 +928,7 @@
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D19" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E19" s="5">
         <v>12</v>
@@ -919,7 +954,7 @@
     </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D20" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E20" s="5">
         <v>14</v>
@@ -945,7 +980,7 @@
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D21" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E21" s="8">
         <v>14</v>
@@ -970,8 +1005,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="G5:K5"/>
+    <mergeCell ref="O5:S5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>